<commit_message>
Updated soil type data
</commit_message>
<xml_diff>
--- a/ISRaD_data_files/Guillet_2010.xlsx
+++ b/ISRaD_data_files/Guillet_2010.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20384"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfromm\Documents\GitHub\ISRaD\ISRaD_data_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB36DA4-47D8-470F-BBA9-2F1294956836}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27840" windowHeight="16660" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27840" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="1054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1831" uniqueCount="1067">
   <si>
     <t>entry_name</t>
   </si>
@@ -3190,12 +3196,51 @@
   </si>
   <si>
     <t>frc_fraction_modern_sd</t>
+  </si>
+  <si>
+    <t>pro_usda_soil_order</t>
+  </si>
+  <si>
+    <t>Alfisols</t>
+  </si>
+  <si>
+    <t>Andisols</t>
+  </si>
+  <si>
+    <t>Aridisols</t>
+  </si>
+  <si>
+    <t>Entisols</t>
+  </si>
+  <si>
+    <t>Gelisols</t>
+  </si>
+  <si>
+    <t>Histosols</t>
+  </si>
+  <si>
+    <t>Inceptisols</t>
+  </si>
+  <si>
+    <t>Mollisols</t>
+  </si>
+  <si>
+    <t>Oxisols</t>
+  </si>
+  <si>
+    <t>Spodosols</t>
+  </si>
+  <si>
+    <t>Ultisols</t>
+  </si>
+  <si>
+    <t>Vertisols</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3326,10 +3371,18 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_layer" xfId="9"/>
+    <cellStyle name="Normal_layer" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3611,16 +3664,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3670,7 +3723,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3717,7 +3770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3755,7 +3808,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3808,20 +3861,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3844,7 +3897,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3867,7 +3920,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3884,7 +3937,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3901,7 +3954,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -3918,7 +3971,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -3947,16 +4000,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AK9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3997,76 +4050,79 @@
         <v>89</v>
       </c>
       <c r="N1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="O1" t="s">
         <v>90</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>91</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>93</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>94</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>95</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>96</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>97</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>98</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>99</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>100</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>101</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>102</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>103</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>104</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>105</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>106</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>107</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>108</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>109</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>110</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>111</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4106,77 +4162,77 @@
       <c r="M2" t="s">
         <v>121</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>122</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>123</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>124</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>125</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>126</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>127</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>128</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>129</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>130</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>131</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>132</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>133</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>134</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>135</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>136</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>137</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>138</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>139</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>140</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>141</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>142</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>143</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4204,29 +4260,26 @@
       <c r="M3" t="s">
         <v>36</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>150</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>151</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>152</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>149</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>153</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>154</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>155</v>
-      </c>
-      <c r="V3" t="s">
-        <v>156</v>
       </c>
       <c r="W3" t="s">
         <v>156</v>
@@ -4235,43 +4288,46 @@
         <v>156</v>
       </c>
       <c r="Y3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z3" t="s">
         <v>157</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>158</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>159</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>160</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>161</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>162</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>153</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>163</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>164</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>165</v>
       </c>
       <c r="AI3" t="s">
         <v>165</v>
       </c>
       <c r="AJ3" t="s">
+        <v>165</v>
+      </c>
+      <c r="AK3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -4285,19 +4341,22 @@
         <v>167</v>
       </c>
       <c r="N4" t="s">
+        <v>1055</v>
+      </c>
+      <c r="O4" t="s">
         <v>168</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>169</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>170</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -4311,19 +4370,22 @@
         <v>167</v>
       </c>
       <c r="N5" t="s">
+        <v>1055</v>
+      </c>
+      <c r="O5" t="s">
         <v>168</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>169</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>170</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -4337,19 +4399,22 @@
         <v>167</v>
       </c>
       <c r="N6" t="s">
+        <v>1064</v>
+      </c>
+      <c r="O6" t="s">
         <v>174</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>169</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>170</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -4363,19 +4428,22 @@
         <v>167</v>
       </c>
       <c r="N7" t="s">
+        <v>1055</v>
+      </c>
+      <c r="O7" t="s">
         <v>168</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>169</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>170</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -4388,17 +4456,17 @@
       <c r="H8" t="s">
         <v>167</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>169</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>170</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -4412,15 +4480,18 @@
         <v>167</v>
       </c>
       <c r="N9" t="s">
+        <v>1055</v>
+      </c>
+      <c r="O9" t="s">
         <v>168</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>169</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>170</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>180</v>
       </c>
     </row>
@@ -4428,6 +4499,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8A31100E-D5FC-4066-93DF-1603B4BDA176}">
+          <x14:formula1>
+            <xm:f>'controlled vocabulary'!$E$4:$E$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>N4:N1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
@@ -4436,14 +4517,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4556,7 +4637,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4666,7 +4747,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4758,19 +4839,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CT60"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BC7" sqref="BC7:BD60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5066,7 +5147,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="2" spans="1:98">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5362,7 +5443,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="3" spans="1:98">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5601,7 +5682,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="4" spans="1:98">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -5633,7 +5714,7 @@
         <v>0.44000000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:98">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -5665,7 +5746,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:98">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -5697,7 +5778,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:98">
+    <row r="7" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -5741,7 +5822,7 @@
         <v>4.0999999999999995E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:98">
+    <row r="8" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -5785,7 +5866,7 @@
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:98">
+    <row r="9" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -5829,7 +5910,7 @@
         <v>4.0999999999999995E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:98">
+    <row r="10" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -5863,7 +5944,7 @@
       <c r="BC10" s="1"/>
       <c r="BD10" s="1"/>
     </row>
-    <row r="11" spans="1:98">
+    <row r="11" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -5897,7 +5978,7 @@
       <c r="BC11" s="1"/>
       <c r="BD11" s="1"/>
     </row>
-    <row r="12" spans="1:98">
+    <row r="12" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -5931,7 +6012,7 @@
       <c r="BC12" s="1"/>
       <c r="BD12" s="1"/>
     </row>
-    <row r="13" spans="1:98">
+    <row r="13" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -5975,7 +6056,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:98">
+    <row r="14" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -6009,7 +6090,7 @@
       <c r="BC14" s="1"/>
       <c r="BD14" s="1"/>
     </row>
-    <row r="15" spans="1:98">
+    <row r="15" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -6053,7 +6134,7 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:98">
+    <row r="16" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -6094,7 +6175,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:56">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -6128,7 +6209,7 @@
       <c r="BC17" s="1"/>
       <c r="BD17" s="1"/>
     </row>
-    <row r="18" spans="1:56">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -6162,7 +6243,7 @@
       <c r="BC18" s="1"/>
       <c r="BD18" s="1"/>
     </row>
-    <row r="19" spans="1:56">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -6206,7 +6287,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:56">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -6247,7 +6328,7 @@
         <v>4.0999999999999995E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:56">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -6291,7 +6372,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:56">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -6325,7 +6406,7 @@
       <c r="BC22" s="1"/>
       <c r="BD22" s="1"/>
     </row>
-    <row r="23" spans="1:56">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -6366,7 +6447,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:56">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -6407,7 +6488,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:56">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -6451,7 +6532,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:56">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -6485,7 +6566,7 @@
       <c r="BC26" s="1"/>
       <c r="BD26" s="1"/>
     </row>
-    <row r="27" spans="1:56">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -6526,7 +6607,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:56">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -6570,7 +6651,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:56">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -6614,7 +6695,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:56">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -6655,7 +6736,7 @@
         <v>4.5000000000000005E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:56">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -6699,7 +6780,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:56">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -6743,7 +6824,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:56">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -6784,7 +6865,7 @@
         <v>4.6999999999999993E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:56">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -6828,7 +6909,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:56">
+    <row r="35" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -6872,7 +6953,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:56">
+    <row r="36" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -6916,7 +6997,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:56">
+    <row r="37" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -6960,7 +7041,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:56">
+    <row r="38" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -7004,7 +7085,7 @@
         <v>5.6999999999999993E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:56">
+    <row r="39" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -7048,7 +7129,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:56">
+    <row r="40" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -7092,7 +7173,7 @@
         <v>5.5000000000000005E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:56">
+    <row r="41" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -7136,7 +7217,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:56">
+    <row r="42" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -7180,7 +7261,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:56">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -7224,7 +7305,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:56">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -7268,7 +7349,7 @@
         <v>5.6000000000000008E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:56">
+    <row r="45" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -7312,7 +7393,7 @@
         <v>6.3E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:56">
+    <row r="46" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -7356,7 +7437,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:56">
+    <row r="47" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -7400,7 +7481,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:56">
+    <row r="48" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -7434,7 +7515,7 @@
       <c r="BC48" s="1"/>
       <c r="BD48" s="1"/>
     </row>
-    <row r="49" spans="1:56">
+    <row r="49" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -7478,7 +7559,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:56">
+    <row r="50" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -7522,7 +7603,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:56">
+    <row r="51" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -7566,7 +7647,7 @@
         <v>4.6999999999999993E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:56">
+    <row r="52" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -7610,7 +7691,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:56">
+    <row r="53" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -7654,7 +7735,7 @@
         <v>4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:56">
+    <row r="54" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -7698,7 +7779,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:56">
+    <row r="55" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>43</v>
       </c>
@@ -7742,7 +7823,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:56">
+    <row r="56" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>43</v>
       </c>
@@ -7786,7 +7867,7 @@
         <v>4.6999999999999993E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:56">
+    <row r="57" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -7830,7 +7911,7 @@
         <v>5.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:56">
+    <row r="58" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>43</v>
       </c>
@@ -7874,7 +7955,7 @@
         <v>4.6999999999999993E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:56">
+    <row r="59" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>43</v>
       </c>
@@ -7918,7 +7999,7 @@
         <v>5.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:56">
+    <row r="60" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -7977,14 +8058,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8070,7 +8151,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -8153,7 +8234,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -8212,16 +8293,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1:AK1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:73" ht="52">
+    <row r="1" spans="1:73" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8442,7 +8523,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="2" spans="1:73">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -8660,7 +8741,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="3" spans="1:73">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -8839,14 +8920,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8938,7 +9019,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -9021,7 +9102,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -9080,14 +9161,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:AS21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>808</v>
       </c>
@@ -9100,128 +9183,128 @@
       <c r="D1" t="s">
         <v>811</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>812</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>813</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>814</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>815</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>816</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>817</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>818</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>819</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>820</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>821</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>822</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>823</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>824</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>825</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>826</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>827</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>828</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>829</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>830</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>831</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>832</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>833</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>834</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>835</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>836</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>837</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>838</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>839</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>840</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>841</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>842</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>843</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>844</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>845</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>846</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>847</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>848</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>849</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>850</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -9235,150 +9318,153 @@
         <v>108</v>
       </c>
       <c r="E2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F2" t="s">
         <v>92</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>96</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>109</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>101</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>102</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>104</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>84</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>186</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>188</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>189</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>190</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>192</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>194</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>195</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>196</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>202</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>279</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>284</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>313</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>263</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>267</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>270</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>852</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>624</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>625</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>626</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>627</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>633</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>763</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>853</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>769</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>771</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>773</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>776</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>666</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>670</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>665</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>667</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>672</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
-      <c r="G3" t="s">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
         <v>854</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>855</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>856</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>855</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AN3" t="s">
         <v>732</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>857</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AQ3" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>859</v>
       </c>
@@ -9392,127 +9478,130 @@
         <v>862</v>
       </c>
       <c r="E4" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F4" t="s">
         <v>169</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>863</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>864</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>865</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>866</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>867</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>167</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>868</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>869</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>870</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>871</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>872</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>873</v>
-      </c>
-      <c r="R4" t="s">
-        <v>861</v>
       </c>
       <c r="S4" t="s">
         <v>861</v>
       </c>
       <c r="T4" t="s">
+        <v>861</v>
+      </c>
+      <c r="U4" t="s">
         <v>874</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>875</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>876</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>877</v>
-      </c>
-      <c r="X4" t="s">
-        <v>861</v>
       </c>
       <c r="Y4" t="s">
         <v>861</v>
       </c>
       <c r="Z4" t="s">
+        <v>861</v>
+      </c>
+      <c r="AA4" t="s">
         <v>878</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>879</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>880</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>869</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>881</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>872</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>882</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>883</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>870</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>884</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>885</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>886</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>887</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AN4" t="s">
         <v>888</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AO4" t="s">
         <v>889</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AP4" t="s">
         <v>890</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AQ4" t="s">
         <v>891</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AR4" t="s">
         <v>861</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AS4" t="s">
         <v>877</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>892</v>
       </c>
@@ -9523,109 +9612,112 @@
         <v>894</v>
       </c>
       <c r="E5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F5" t="s">
         <v>895</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>896</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>897</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>898</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>899</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>900</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>901</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>902</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>903</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>904</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>905</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>906</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>907</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>908</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>909</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>910</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>911</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>912</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>913</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>903</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>914</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>906</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>915</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>916</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>904</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>917</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>918</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>919</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>920</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>921</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>922</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>923</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AQ5" t="s">
         <v>924</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AS5" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>925</v>
       </c>
@@ -9636,447 +9728,477 @@
         <v>926</v>
       </c>
       <c r="E6" t="s">
+        <v>1057</v>
+      </c>
+      <c r="F6" t="s">
         <v>927</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>170</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>928</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>929</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>930</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>931</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>932</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>933</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>934</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>935</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>936</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>662</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>937</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>938</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>939</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>940</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>941</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>942</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>933</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>936</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>943</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>944</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>945</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>946</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>927</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>947</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>948</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>949</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>36</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AS6" t="s">
         <v>940</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>950</v>
       </c>
       <c r="B7" t="s">
         <v>951</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
+        <v>1058</v>
+      </c>
+      <c r="G7" t="s">
         <v>952</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>953</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>954</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>955</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>956</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>957</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>958</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>959</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>960</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>961</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>962</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>963</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>957</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>959</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AG7" t="s">
         <v>964</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>965</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>966</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AN7" t="s">
         <v>967</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AO7" t="s">
         <v>968</v>
       </c>
-      <c r="AO7" t="s">
+      <c r="AP7" t="s">
         <v>969</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AQ7" t="s">
         <v>970</v>
       </c>
-      <c r="AR7" t="s">
+      <c r="AS7" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>971</v>
       </c>
       <c r="B8" t="s">
         <v>972</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
+        <v>1059</v>
+      </c>
+      <c r="G8" t="s">
         <v>973</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>974</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>975</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>976</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>977</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>978</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>979</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>980</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>981</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>982</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>983</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>927</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>978</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>980</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AH8" t="s">
         <v>984</v>
       </c>
-      <c r="AM8" t="s">
+      <c r="AN8" t="s">
         <v>985</v>
       </c>
-      <c r="AN8" t="s">
+      <c r="AO8" t="s">
         <v>986</v>
       </c>
-      <c r="AO8" t="s">
+      <c r="AP8" t="s">
         <v>987</v>
       </c>
-      <c r="AP8" t="s">
+      <c r="AQ8" t="s">
         <v>662</v>
       </c>
-      <c r="AR8" t="s">
+      <c r="AS8" t="s">
         <v>927</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>988</v>
       </c>
       <c r="B9" t="s">
         <v>989</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G9" t="s">
         <v>990</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>991</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>992</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>993</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>994</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>995</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>996</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>997</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>998</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AF9" t="s">
         <v>999</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AH9" t="s">
         <v>995</v>
       </c>
-      <c r="AM9" t="s">
+      <c r="AN9" t="s">
         <v>1000</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AO9" t="s">
         <v>1001</v>
       </c>
-      <c r="AO9" t="s">
+      <c r="AP9" t="s">
         <v>1002</v>
       </c>
-      <c r="AP9" t="s">
+      <c r="AQ9" t="s">
         <v>1003</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1004</v>
       </c>
       <c r="B10" t="s">
         <v>1005</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" t="s">
+        <v>1061</v>
+      </c>
+      <c r="G10" t="s">
         <v>1006</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>1007</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>1008</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>1009</v>
       </c>
-      <c r="AM10" t="s">
+      <c r="AN10" t="s">
         <v>1010</v>
       </c>
-      <c r="AN10" t="s">
+      <c r="AO10" t="s">
         <v>1011</v>
       </c>
-      <c r="AO10" t="s">
+      <c r="AP10" t="s">
         <v>1012</v>
       </c>
-      <c r="AP10" t="s">
+      <c r="AQ10" t="s">
         <v>1013</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>1014</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" t="s">
+        <v>1062</v>
+      </c>
+      <c r="G11" t="s">
         <v>1015</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>1016</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>1017</v>
       </c>
-      <c r="AM11" t="s">
+      <c r="AN11" t="s">
         <v>1018</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>1019</v>
       </c>
       <c r="AO11" t="s">
         <v>1019</v>
       </c>
       <c r="AP11" t="s">
+        <v>1019</v>
+      </c>
+      <c r="AQ11" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
-      <c r="H12" t="s">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I12" t="s">
         <v>1021</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>1022</v>
       </c>
-      <c r="AM12" t="s">
+      <c r="AN12" t="s">
         <v>1023</v>
       </c>
-      <c r="AN12" t="s">
+      <c r="AO12" t="s">
         <v>1024</v>
       </c>
-      <c r="AO12" t="s">
+      <c r="AP12" t="s">
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
-      <c r="U13" t="s">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>1064</v>
+      </c>
+      <c r="V13" t="s">
         <v>1026</v>
       </c>
-      <c r="AM13" t="s">
+      <c r="AN13" t="s">
         <v>1027</v>
       </c>
-      <c r="AN13" t="s">
+      <c r="AO13" t="s">
         <v>1028</v>
       </c>
-      <c r="AO13" t="s">
+      <c r="AP13" t="s">
         <v>1029</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
-      <c r="U14" t="s">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>1065</v>
+      </c>
+      <c r="V14" t="s">
         <v>1030</v>
       </c>
-      <c r="AN14" t="s">
+      <c r="AO14" t="s">
         <v>1031</v>
       </c>
-      <c r="AO14" t="s">
+      <c r="AP14" t="s">
         <v>1032</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
-      <c r="U15" t="s">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>1066</v>
+      </c>
+      <c r="V15" t="s">
         <v>1033</v>
       </c>
-      <c r="AN15" t="s">
+      <c r="AO15" t="s">
         <v>1034</v>
       </c>
-      <c r="AO15" t="s">
+      <c r="AP15" t="s">
         <v>1035</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
-      <c r="U16" t="s">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="V16" t="s">
         <v>1036</v>
       </c>
-      <c r="AN16" t="s">
+      <c r="AO16" t="s">
         <v>1037</v>
       </c>
-      <c r="AO16" t="s">
+      <c r="AP16" t="s">
         <v>1038</v>
       </c>
     </row>
-    <row r="17" spans="40:41">
-      <c r="AN17" t="s">
+    <row r="17" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO17" t="s">
         <v>1039</v>
       </c>
-      <c r="AO17" t="s">
+      <c r="AP17" t="s">
         <v>1040</v>
       </c>
     </row>
-    <row r="18" spans="40:41">
-      <c r="AN18" t="s">
+    <row r="18" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO18" t="s">
         <v>1041</v>
       </c>
-      <c r="AO18" t="s">
+      <c r="AP18" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="19" spans="40:41">
-      <c r="AN19" t="s">
+    <row r="19" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO19" t="s">
         <v>1043</v>
       </c>
-      <c r="AO19" t="s">
+      <c r="AP19" t="s">
         <v>1044</v>
       </c>
     </row>
-    <row r="20" spans="40:41">
-      <c r="AN20" t="s">
+    <row r="20" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO20" t="s">
         <v>1045</v>
       </c>
-      <c r="AO20" t="s">
+      <c r="AP20" t="s">
         <v>1046</v>
       </c>
     </row>
-    <row r="21" spans="40:41">
-      <c r="AN21" t="s">
+    <row r="21" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO21" t="s">
         <v>1047</v>
       </c>
     </row>

</xml_diff>